<commit_message>
working on the feature -- amazon product
</commit_message>
<xml_diff>
--- a/data/settings/keywords.xlsx
+++ b/data/settings/keywords.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sss</t>
+          <t>skdslkf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sssa</t>
+          <t>skdsl</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sasd</t>
+          <t>skdfjl</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>slkdf</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>skeks</t>
         </is>
       </c>
     </row>

</xml_diff>